<commit_message>
testdata examples and testpoints redone
</commit_message>
<xml_diff>
--- a/inst/testdata/latlon/testpoints_10.xlsx
+++ b/inst/testdata/latlon/testpoints_10.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,313 +360,183 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>lat</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>lon</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>siteid</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>lat</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>lon</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>REGISTRY_ID</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>PRIMARY_NAME</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>NAICS</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>SIC</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>PGM_SYS_ACRNMS</t>
+          <t>sitename</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2">
+        <v>47.22107</v>
+      </c>
+      <c r="B2">
+        <v>-122.01626</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>32.333812</v>
-      </c>
-      <c r="C2">
-        <v>-90.16603499999999</v>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>110012157520</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
           <t>Example name for site 1</t>
         </is>
-      </c>
-      <c r="F2">
-        <v>722410</v>
-      </c>
-      <c r="G2">
-        <v>5992</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
+        <v>40.227778</v>
+      </c>
+      <c r="B3">
+        <v>-76.825833</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>43.330894</v>
-      </c>
-      <c r="C3">
-        <v>-75.746979</v>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>110020822671</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
           <t>Example name for site 2</t>
         </is>
-      </c>
-      <c r="F3">
-        <v>722410</v>
-      </c>
-      <c r="G3">
-        <v>5992</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
+        <v>41.0697</v>
+      </c>
+      <c r="B4">
+        <v>-112.04539</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>43.40934</v>
-      </c>
-      <c r="C4">
-        <v>-83.90703999999999</v>
-      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>110021850558</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
           <t>Example name for site 3</t>
         </is>
-      </c>
-      <c r="F4">
-        <v>722410</v>
-      </c>
-      <c r="G4">
-        <v>5992</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
+        <v>39.438169</v>
+      </c>
+      <c r="B5">
+        <v>-123.78846</v>
+      </c>
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>42.44731</v>
-      </c>
-      <c r="C5">
-        <v>-83.08396</v>
-      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>110022674319</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
           <t>Example name for site 4</t>
         </is>
-      </c>
-      <c r="F5">
-        <v>722410</v>
-      </c>
-      <c r="G5">
-        <v>5992</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
+        <v>33.157147</v>
+      </c>
+      <c r="B6">
+        <v>-97.12994399999999</v>
+      </c>
+      <c r="C6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>40.571495</v>
-      </c>
-      <c r="C6">
-        <v>-104.507025</v>
-      </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>110022693307</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
           <t>Example name for site 5</t>
         </is>
-      </c>
-      <c r="F6">
-        <v>722410</v>
-      </c>
-      <c r="G6">
-        <v>5992</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
+        <v>40.90765</v>
+      </c>
+      <c r="B7">
+        <v>-73.84775999999999</v>
+      </c>
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>41.85192</v>
-      </c>
-      <c r="C7">
-        <v>-87.86230999999999</v>
-      </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>110022742264</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
           <t>Example name for site 6</t>
         </is>
-      </c>
-      <c r="F7">
-        <v>722410</v>
-      </c>
-      <c r="G7">
-        <v>5992</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
+        <v>40.21152</v>
+      </c>
+      <c r="B8">
+        <v>-109.23989</v>
+      </c>
+      <c r="C8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>40.784872</v>
-      </c>
-      <c r="C8">
-        <v>-73.948553</v>
-      </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>110022742282</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
           <t>Example name for site 7</t>
         </is>
-      </c>
-      <c r="F8">
-        <v>722410</v>
-      </c>
-      <c r="G8">
-        <v>5992</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
+        <v>29.49421</v>
+      </c>
+      <c r="B9">
+        <v>-81.67028000000001</v>
+      </c>
+      <c r="C9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>36.02956</v>
-      </c>
-      <c r="C9">
-        <v>-95.90336000000001</v>
-      </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>110022742308</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
           <t>Example name for site 8</t>
         </is>
-      </c>
-      <c r="F9">
-        <v>722410</v>
-      </c>
-      <c r="G9">
-        <v>5992</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
+        <v>43.29147</v>
+      </c>
+      <c r="B10">
+        <v>-95.15028</v>
+      </c>
+      <c r="C10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>40.38978</v>
-      </c>
-      <c r="C10">
-        <v>-122.28185</v>
-      </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>110030905858</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
           <t>Example name for site 9</t>
         </is>
-      </c>
-      <c r="F10">
-        <v>722410</v>
-      </c>
-      <c r="G10">
-        <v>5992</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
+        <v>39.058005</v>
+      </c>
+      <c r="B11">
+        <v>-104.854929</v>
+      </c>
+      <c r="C11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>41.13597</v>
-      </c>
-      <c r="C11">
-        <v>-72.30355</v>
-      </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>110032375873</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
           <t>Example name for site 10</t>
         </is>
-      </c>
-      <c r="F11">
-        <v>722410</v>
-      </c>
-      <c r="G11">
-        <v>5992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced all test data inputs and outputs and documentation
</commit_message>
<xml_diff>
--- a/inst/testdata/latlon/testpoints_10.xlsx
+++ b/inst/testdata/latlon/testpoints_10.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="varname" sheetId="1" r:id="rId1"/>
+    <sheet name="testpoints" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -381,161 +381,161 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>47.22107</v>
+        <v>40.81417</v>
       </c>
       <c r="B2">
-        <v>-122.01626</v>
+        <v>-96.69963</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Example name for site 1</t>
+          <t>Example Site 1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>40.227778</v>
+        <v>33.74774</v>
       </c>
       <c r="B3">
-        <v>-76.825833</v>
+        <v>-116.927828</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Example name for site 2</t>
+          <t>Example Site 2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>41.0697</v>
+        <v>37.2335</v>
       </c>
       <c r="B4">
-        <v>-112.04539</v>
+        <v>-112.8752</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Example name for site 3</t>
+          <t>Example Site 3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>39.438169</v>
+        <v>30.2775</v>
       </c>
       <c r="B5">
-        <v>-123.78846</v>
+        <v>-97.82528000000001</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Example name for site 4</t>
+          <t>Example Site 4</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>33.157147</v>
+        <v>31.346534</v>
       </c>
       <c r="B6">
-        <v>-97.12994399999999</v>
+        <v>-92.401505</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Example name for site 5</t>
+          <t>Example Site 5</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>40.90765</v>
+        <v>39.45225</v>
       </c>
       <c r="B7">
-        <v>-73.84775999999999</v>
+        <v>-80.13771</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Example name for site 6</t>
+          <t>Example Site 6</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>40.21152</v>
+        <v>33.437222</v>
       </c>
       <c r="B8">
-        <v>-109.23989</v>
+        <v>-86.7375</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Example name for site 7</t>
+          <t>Example Site 7</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>29.49421</v>
+        <v>29.564069</v>
       </c>
       <c r="B9">
-        <v>-81.67028000000001</v>
+        <v>-98.191041</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Example name for site 8</t>
+          <t>Example Site 8</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>43.29147</v>
+        <v>38.603834</v>
       </c>
       <c r="B10">
-        <v>-95.15028</v>
+        <v>-121.46303</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Example name for site 9</t>
+          <t>Example Site 9</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>39.058005</v>
+        <v>39.27679</v>
       </c>
       <c r="B11">
-        <v>-104.854929</v>
+        <v>-84.41392999999999</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Example name for site 10</t>
+          <t>Example Site 10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated testoutputs, testpoints etc
</commit_message>
<xml_diff>
--- a/inst/testdata/latlon/testpoints_10.xlsx
+++ b/inst/testdata/latlon/testpoints_10.xlsx
@@ -370,7 +370,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>siteid</t>
+          <t>sitenumber</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -381,10 +381,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>40.81417</v>
+        <v>43.21166</v>
       </c>
       <c r="B2">
-        <v>-96.69963</v>
+        <v>-76.28693800000001</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -397,10 +397,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>33.74774</v>
+        <v>32.75469</v>
       </c>
       <c r="B3">
-        <v>-116.927828</v>
+        <v>-96.77826</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -413,10 +413,10 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>37.2335</v>
+        <v>39.118211</v>
       </c>
       <c r="B4">
-        <v>-112.8752</v>
+        <v>-94.93859</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -429,10 +429,10 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>30.2775</v>
+        <v>39.736799</v>
       </c>
       <c r="B5">
-        <v>-97.82528000000001</v>
+        <v>-105.07198</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -445,10 +445,10 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>31.346534</v>
+        <v>30.45373</v>
       </c>
       <c r="B6">
-        <v>-92.401505</v>
+        <v>-89.01851000000001</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -461,10 +461,10 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>39.45225</v>
+        <v>44.07253</v>
       </c>
       <c r="B7">
-        <v>-80.13771</v>
+        <v>-123.06642</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -477,10 +477,10 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>33.437222</v>
+        <v>35.704882</v>
       </c>
       <c r="B8">
-        <v>-86.7375</v>
+        <v>-81.31295900000001</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -493,10 +493,10 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>29.564069</v>
+        <v>18.05673</v>
       </c>
       <c r="B9">
-        <v>-98.191041</v>
+        <v>-66.72190999999999</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -509,10 +509,10 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>38.603834</v>
+        <v>41.953372</v>
       </c>
       <c r="B10">
-        <v>-121.46303</v>
+        <v>-87.68844</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -525,10 +525,10 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>39.27679</v>
+        <v>39.735207</v>
       </c>
       <c r="B11">
-        <v>-84.41392999999999</v>
+        <v>-86.140005</v>
       </c>
       <c r="C11">
         <v>10</v>

</xml_diff>

<commit_message>
recreate testpoints and testoutput files
</commit_message>
<xml_diff>
--- a/inst/testdata/latlon/testpoints_10.xlsx
+++ b/inst/testdata/latlon/testpoints_10.xlsx
@@ -381,10 +381,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>43.21166</v>
+        <v>39.74649</v>
       </c>
       <c r="B2">
-        <v>-76.28693800000001</v>
+        <v>-74.20121</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -397,10 +397,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>32.75469</v>
+        <v>39.78107</v>
       </c>
       <c r="B3">
-        <v>-96.77826</v>
+        <v>-104.91286</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -413,10 +413,10 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>39.118211</v>
+        <v>35.47007</v>
       </c>
       <c r="B4">
-        <v>-94.93859</v>
+        <v>-82.87474</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -429,10 +429,10 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>39.736799</v>
+        <v>46.8304</v>
       </c>
       <c r="B5">
-        <v>-105.07198</v>
+        <v>-100.77309</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -445,10 +445,10 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>30.45373</v>
+        <v>43.81283</v>
       </c>
       <c r="B6">
-        <v>-89.01851000000001</v>
+        <v>-94.07801000000001</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -461,10 +461,10 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>44.07253</v>
+        <v>18.33551</v>
       </c>
       <c r="B7">
-        <v>-123.06642</v>
+        <v>-64.9636</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -477,10 +477,10 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>35.704882</v>
+        <v>31.414179</v>
       </c>
       <c r="B8">
-        <v>-81.31295900000001</v>
+        <v>-103.514546</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -493,10 +493,10 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>18.05673</v>
+        <v>39.74874</v>
       </c>
       <c r="B9">
-        <v>-66.72190999999999</v>
+        <v>-84.16482000000001</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -509,10 +509,10 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>41.953372</v>
+        <v>26.065681</v>
       </c>
       <c r="B10">
-        <v>-87.68844</v>
+        <v>-80.23483400000001</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -525,10 +525,10 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>39.735207</v>
+        <v>36.776494</v>
       </c>
       <c r="B11">
-        <v>-86.140005</v>
+        <v>-114.03794</v>
       </c>
       <c r="C11">
         <v>10</v>

</xml_diff>

<commit_message>
redo testpoints etc., work on testing groups of functions, remove testpoints_conus5 , etc. (#443)
</commit_message>
<xml_diff>
--- a/inst/testdata/latlon/testpoints_10.xlsx
+++ b/inst/testdata/latlon/testpoints_10.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -373,170 +373,115 @@
           <t>sitenumber</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>sitename</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>39.74649</v>
+        <v>30.977402</v>
       </c>
       <c r="B2">
-        <v>-74.20121</v>
+        <v>-83.36899699999999</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Example Site 1</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>39.78107</v>
+        <v>32.515813</v>
       </c>
       <c r="B3">
-        <v>-104.91286</v>
+        <v>-86.377325</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Example Site 2</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>35.47007</v>
+        <v>42.23498</v>
       </c>
       <c r="B4">
-        <v>-82.87474</v>
+        <v>-88.30540999999999</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Example Site 3</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>46.8304</v>
+        <v>33.870013</v>
       </c>
       <c r="B5">
-        <v>-100.77309</v>
+        <v>-118.377777</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Example Site 4</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>43.81283</v>
+        <v>34.014929</v>
       </c>
       <c r="B6">
-        <v>-94.07801000000001</v>
+        <v>-118.205387</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Example Site 5</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>18.33551</v>
+        <v>40.731099</v>
       </c>
       <c r="B7">
-        <v>-64.9636</v>
+        <v>-74.173067</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Example Site 6</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>31.414179</v>
+        <v>37.81144</v>
       </c>
       <c r="B8">
-        <v>-103.514546</v>
+        <v>-121.29348</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Example Site 7</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>39.74874</v>
+        <v>44.85387</v>
       </c>
       <c r="B9">
-        <v>-84.16482000000001</v>
+        <v>-93.04713</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Example Site 8</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>26.065681</v>
+        <v>41.18661</v>
       </c>
       <c r="B10">
-        <v>-80.23483400000001</v>
+        <v>-111.94904</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Example Site 9</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>36.776494</v>
+        <v>40.71239</v>
       </c>
       <c r="B11">
-        <v>-114.03794</v>
+        <v>-74.5847</v>
       </c>
       <c r="C11">
         <v>10</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Example Site 10</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>